<commit_message>
Minor updates to files for indents and typos
</commit_message>
<xml_diff>
--- a/uml_diagram.xlsx
+++ b/uml_diagram.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevemaddison/Documents/CodeClan/Module 1 Project - Travel Bucket List/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevemaddison/codeclan_work/module_1_project_travelbucket/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D764FA8-A094-9041-B34F-EB600F1A4834}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228D0865-A783-2342-B35E-A49EDB83554E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14500" xr2:uid="{B9204630-62A2-1F4E-BA6E-238F381DEFCA}"/>
   </bookViews>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
-  <si>
-    <t>ID (auto)</t>
-  </si>
-  <si>
-    <t>country_id (int)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>name (string)</t>
   </si>
@@ -93,38 +87,44 @@
     <t>self.delete_al()</t>
   </si>
   <si>
-    <t>UML Diagram - MVP</t>
-  </si>
-  <si>
-    <t>find_countries_not_visited(country_visited)</t>
-  </si>
-  <si>
-    <t>find_countries_visited(country_visited)</t>
-  </si>
-  <si>
-    <t>find_cities_not_visited(city_visited)</t>
-  </si>
-  <si>
-    <t>find_cities_visited(city_visited)</t>
-  </si>
-  <si>
-    <t>country_visited (string)</t>
-  </si>
-  <si>
-    <t>city_visited (string)</t>
-  </si>
-  <si>
-    <t>&lt;= class method?</t>
-  </si>
-  <si>
-    <t>"Yes" if any city has been visited</t>
+    <t>find countries visited</t>
+  </si>
+  <si>
+    <t>find countries not visited</t>
+  </si>
+  <si>
+    <t>find cities visited</t>
+  </si>
+  <si>
+    <t>find cities not visited</t>
+  </si>
+  <si>
+    <t>country_visited (boolean)</t>
+  </si>
+  <si>
+    <t>city_visited (boolean)</t>
+  </si>
+  <si>
+    <t>UML Diagram</t>
+  </si>
+  <si>
+    <t>rating (string)</t>
+  </si>
+  <si>
+    <t>id (auto)</t>
+  </si>
+  <si>
+    <t>country_id (int) - joins to country.id</t>
+  </si>
+  <si>
+    <t>review (text)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -134,6 +134,14 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -213,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -222,12 +230,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,226 +549,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A0A1CAE-1299-EA4B-913E-34C412F126EA}">
-  <dimension ref="A2:F24"/>
+  <dimension ref="B2:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
     <col min="5" max="5" width="33.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="12"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="E6" s="3" t="s">
+      <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="E7" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C10" s="4"/>
+      <c r="E10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="5"/>
-      <c r="C9" s="7"/>
-      <c r="E9" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="10" t="s">
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C15" s="4"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C16" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C17" s="4" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="4"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="4"/>
-      <c r="C18" s="7"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C18" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="12"/>
+      <c r="E18" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C19" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="D19" s="7"/>
-      <c r="E19" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="4" t="s">
+      <c r="E19" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C20" s="4"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C23" s="4"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C24" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C25" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C26" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="4"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="6" t="s">
+      <c r="D26" s="7"/>
+      <c r="E26" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="9" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>